<commit_message>
templates/Surgery/Operatørvurdering.v1.oet: oppdatert template med all viktig innhold , occurancy osv., mangler kodeverk fra DIPS surgery/Operasjon-forms - behov for logikk.xlsx: oppdtert med info om templates/Surgery/Operatørvurdering.v1.oet
</commit_message>
<xml_diff>
--- a/surgery/Operasjon-forms - behov for logikk.xlsx
+++ b/surgery/Operasjon-forms - behov for logikk.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Operasjonslanlegging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahe\dips-ckm\surgery\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
   <si>
     <t>Arketype</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>Problem/diagnose</t>
-  </si>
-  <si>
-    <t>BNA</t>
   </si>
   <si>
     <t>Felt/element</t>
@@ -129,9 +126,6 @@
     <t>Operasjonsdetaljer</t>
   </si>
   <si>
-    <t>Operasjonleie</t>
-  </si>
-  <si>
     <t>Må være mulighet å kun fylle inn timer eller minutter. Gjennomsnittsknivtid legges inn som default.</t>
   </si>
   <si>
@@ -146,6 +140,45 @@
   <si>
     <t>Hjelpetekst skal vises i tolltipp (finnes i template i annotations).
 Kn vi fjerne radioknappen med ikke valgt i formen? Vet ikke hvordan det gjøres:) Hvis ikke det er mulig må vi heller ha det som kombobox.</t>
+  </si>
+  <si>
+    <t>Avdekning/incisjon</t>
+  </si>
+  <si>
+    <t>Legge inn link til tilsvarende dokument i DocMap (Ståle skulle underøke, håper det er avklart nå?)</t>
+  </si>
+  <si>
+    <t>BNAMGR</t>
+  </si>
+  <si>
+    <t>BNA/MGR</t>
+  </si>
+  <si>
+    <t>Antibiotikaprofylakse</t>
+  </si>
+  <si>
+    <t>Kan vi få en link til nasjonal veileder</t>
+  </si>
+  <si>
+    <t>Tromsboseprofylakse</t>
+  </si>
+  <si>
+    <t>Spesille behov for kirurgi</t>
+  </si>
+  <si>
+    <t>Alle elementer som er brukt</t>
+  </si>
+  <si>
+    <t>Re-use. Gjenbruk informasjon fra beslutningsnotat.</t>
+  </si>
+  <si>
+    <t>Medikamenter ved krirugi</t>
+  </si>
+  <si>
+    <t>Tilleggsinformasjon kirurgi</t>
+  </si>
+  <si>
+    <t>Asa fysisk status klassifikasjon</t>
   </si>
 </sst>
 </file>
@@ -477,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -517,152 +550,225 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>34</v>
+      <c r="D13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
openEHR-EHR-CLUSTER.bodypart.v1.adl: ny tatt inn og oversatt til no openEHR-EHR-OBSERVATION.exam.v1.adl: importert norsk versjon fra arketyper.no og lagt til og oversatt til no openEHR-EHR-OBSERVATION.organ_status_evaluation_surgery.v1.adl: gjort endring, lagt til et cluster for detaljer. templates/Surgery/Anestesi previsitt.oet:mangler koder for postop overvåking ofg spesialutstyr, eller ferdig. templates/Surgery/Operatørvurdering.v1.oet: Ferdig etter siste arketype oppdatering. Lagt til openEHR-EHR-CLUSTER.bodypart.v1.adl  bodyprt og fjernet "auskultasjon"
</commit_message>
<xml_diff>
--- a/surgery/Operasjon-forms - behov for logikk.xlsx
+++ b/surgery/Operasjon-forms - behov for logikk.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
   <si>
     <t>Arketype</t>
   </si>
@@ -148,16 +148,67 @@
     <t>Spesielle behov for kirurgi</t>
   </si>
   <si>
-    <t>Skal ikke vises fra start, kun mulighet å legge til (som diagnose)</t>
-  </si>
-  <si>
-    <t>Undersøkelse</t>
-  </si>
-  <si>
-    <t>Auskultasjon thorax</t>
-  </si>
-  <si>
-    <t>Skal ikke vises fra start, mulighet til å legge til og velge f.eks. legg til asukultasjon hjerte, legg til auskultasjon lunge etc. Velge fra en nedtrekksmeny?</t>
+    <t>Anestesi previsitt</t>
+  </si>
+  <si>
+    <t>Høyde</t>
+  </si>
+  <si>
+    <t>Vekt</t>
+  </si>
+  <si>
+    <t>NYHA</t>
+  </si>
+  <si>
+    <t>Hjertesvikt klassifikasjon</t>
+  </si>
+  <si>
+    <t>Legg til forklaring i tooltipp som hjelpetekst</t>
+  </si>
+  <si>
+    <t>Helserisiko annet</t>
+  </si>
+  <si>
+    <t>Risikofaktor</t>
+  </si>
+  <si>
+    <t>Helserisiko medikamenter</t>
+  </si>
+  <si>
+    <t>Medikament</t>
+  </si>
+  <si>
+    <t>Evaluering anestesi previsitt</t>
+  </si>
+  <si>
+    <t>Re-use. Gjenbruk informasjon fra saken (siste verdi).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-use. Gjenbruk informasjon fra saken (sdiste verdi). </t>
+  </si>
+  <si>
+    <t>Generell reuse</t>
+  </si>
+  <si>
+    <t>Det må vises at informasjonen er innhentet fra en annen plass f.eks. grået ut?</t>
+  </si>
+  <si>
+    <t>Re-use. Dersom medikament er registrert i operatørvurdering skal det vises som risikofaktor. Er det mulig i fase 1? Hvordan?</t>
+  </si>
+  <si>
+    <t>Re-use. Dersom røyking status er satt på røyker skal det vises som risikofaktor? Er det mulig i fase 1? Hvordan?</t>
+  </si>
+  <si>
+    <t>Undersøkelse hjerte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skal ikke vises fra start, mulighet til å legge til </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skal ikke vises fra start, kun mulighet å legge til </t>
+  </si>
+  <si>
+    <t>Undersøkelse lunge</t>
   </si>
 </sst>
 </file>
@@ -510,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,29 +766,124 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="C18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
openEHR-EHR-OBSERVATION.body_weight.v1.adl: feilmelding ved export til OPT
</commit_message>
<xml_diff>
--- a/surgery/Operasjon-forms - behov for logikk.xlsx
+++ b/surgery/Operasjon-forms - behov for logikk.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
   <si>
     <t>Arketype</t>
   </si>
@@ -59,12 +59,6 @@
     <t>Gjennomsnitts knivtid</t>
   </si>
   <si>
-    <t>Omsorgsnivå</t>
-  </si>
-  <si>
-    <t>Lokalisering/behandlingssted</t>
-  </si>
-  <si>
     <t>ASA fysisk status klassifikasjon</t>
   </si>
   <si>
@@ -77,18 +71,12 @@
     <t>Hastegrad detaljer</t>
   </si>
   <si>
-    <t>Beregnet tidsfrist øhj</t>
-  </si>
-  <si>
     <t>Skal pasienten på operasjonsprogrammet i dag?</t>
   </si>
   <si>
     <t>Procedure request</t>
   </si>
   <si>
-    <t>Skal ikke vises i skjema, kun mulighet til å legge til. Kun diagnose feltet skal vises, ingenting av de andre.</t>
-  </si>
-  <si>
     <t>Operatørvurdering</t>
   </si>
   <si>
@@ -120,15 +108,6 @@
   </si>
   <si>
     <t>Tilleggsinformasjon kirurgi</t>
-  </si>
-  <si>
-    <t>Regens ut automatisk avhengig av valg.</t>
-  </si>
-  <si>
-    <t>Dersom Harstad blir med i piloten må det legges inn rett kodeverk her. For mange kodeverk i DIPS admin, jeg fant ikke den rette. Helge vet sikkert bedre. (Det må være Harstad, Narvik, Tromsø)</t>
-  </si>
-  <si>
-    <t>Read only. Verdier må hentes fra classic og vises her, avhengig av prosedyretype</t>
   </si>
   <si>
     <t>Hjelpetekst skal vises i tolltipp:
@@ -136,9 +115,6 @@
 Svar Nei for å la inntakskoordinator/kontor sette pasienten inn på operasjonsprogrammet innenfor den tidsrammen som du har satt.</t>
   </si>
   <si>
-    <t>Senest dato fro ønsket service</t>
-  </si>
-  <si>
     <t>Ved øhj kalkureres dette ut ifra satt verdi for ønsket gjennomført innen</t>
   </si>
   <si>
@@ -187,9 +163,6 @@
     <t xml:space="preserve">Re-use. Gjenbruk informasjon fra saken (sdiste verdi). </t>
   </si>
   <si>
-    <t>Generell reuse</t>
-  </si>
-  <si>
     <t>Det må vises at informasjonen er innhentet fra en annen plass f.eks. grået ut?</t>
   </si>
   <si>
@@ -209,13 +182,46 @@
   </si>
   <si>
     <t>Undersøkelse lunge</t>
+  </si>
+  <si>
+    <t>Annet/generelt:</t>
+  </si>
+  <si>
+    <t>Re-use</t>
+  </si>
+  <si>
+    <t>Duration felt</t>
+  </si>
+  <si>
+    <t>Får vi til å skrive inn 3t, 2d etc. istendefor å vise alle små fletene som må fylles ut?</t>
+  </si>
+  <si>
+    <t>Beregnet tidsfrist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skal ikke vises i skjema, kun mulighet til å legge til. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hele Fieldset </t>
+  </si>
+  <si>
+    <t>Ønsket helsepsersonell</t>
+  </si>
+  <si>
+    <t>Navngitt behandler</t>
+  </si>
+  <si>
+    <t>Kan dette fremheves på en måte når det er avkrysset for obliagtorisk?</t>
+  </si>
+  <si>
+    <t>Verdier må hentes fra classic og vises her, avhengig av prosedyretype</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +233,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -252,7 +271,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -260,11 +279,146 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -272,13 +426,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -287,6 +495,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -561,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,7 +789,7 @@
     <col min="5" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -594,297 +807,342 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+      <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="8"/>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="D9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="C17" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="16"/>
+      <c r="B18" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="16"/>
+      <c r="B19" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="16"/>
+      <c r="B21" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="D21" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="16"/>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+    </row>
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="2" t="s">
+    </row>
+    <row r="24" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="21"/>
+      <c r="B24" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>28</v>
+      <c r="E24" s="23" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
openEHR-EHR-CLUSTER.important_information_procedure.v1.adl:tatt inn reservasjoner og så fjernet igjen openEHR-EHR-OBSERVATION.surgery_details.v1.adl: fjernet reservasjoner, brukes sjekk list istedenfor templates/Surgery/Operatørvurdering.v2.oet: ny template med sjekklist for allergier istedenfor overfølsometsreaksjner og reseravsjoner som sjekkliste arketype
</commit_message>
<xml_diff>
--- a/surgery/Operasjon-forms - behov for logikk.xlsx
+++ b/surgery/Operasjon-forms - behov for logikk.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
   <si>
     <t>Arketype</t>
   </si>
@@ -124,12 +124,6 @@
     <t>Spesielle behov for kirurgi</t>
   </si>
   <si>
-    <t>Anestesi previsitt</t>
-  </si>
-  <si>
-    <t>Høyde</t>
-  </si>
-  <si>
     <t>Vekt</t>
   </si>
   <si>
@@ -172,12 +166,6 @@
     <t>Re-use. Dersom røyking status er satt på røyker skal det vises som risikofaktor? Er det mulig i fase 1? Hvordan?</t>
   </si>
   <si>
-    <t>Undersøkelse hjerte</t>
-  </si>
-  <si>
-    <t>Undersøkelse lunge</t>
-  </si>
-  <si>
     <t>Annet/generelt:</t>
   </si>
   <si>
@@ -220,10 +208,31 @@
     <t>Kan dette vises slik: syst/diast mmHg?</t>
   </si>
   <si>
-    <t>US. funn</t>
-  </si>
-  <si>
-    <t>Skal kun vises når det er avkrysset for normal eller avvik</t>
+    <t>alt</t>
+  </si>
+  <si>
+    <t>Forcwe min. multiplicity virker ikke. Ønsker at det kun vises som legg til felt.</t>
+  </si>
+  <si>
+    <t>Force min multiplicity</t>
+  </si>
+  <si>
+    <t>Får vi dette til å virke også på cluster nivå? Virker ikke nå.</t>
+  </si>
+  <si>
+    <t>Allergi i versjon 4</t>
+  </si>
+  <si>
+    <t>Allergi med betydning i versjon 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beskrivelse </t>
+  </si>
+  <si>
+    <t>Skal kun vises dersom ja er valgt</t>
+  </si>
+  <si>
+    <t>Reservasjoner med betydning i versjon 5</t>
   </si>
 </sst>
 </file>
@@ -261,7 +270,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.34998626667073579"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -504,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -560,43 +569,40 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -884,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -917,124 +923,124 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="16"/>
+      <c r="B3" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
+      <c r="B4" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="22"/>
-      <c r="B3" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="24" t="s">
+      <c r="D5" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23" t="s">
+      <c r="E5" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="16"/>
+      <c r="B7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="16"/>
+      <c r="B8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="24"/>
+      <c r="B9" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="22"/>
-      <c r="B6" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
-      <c r="B7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="22"/>
-      <c r="B8" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="29"/>
-      <c r="B9" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="26" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1103,75 +1109,73 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="14" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8"/>
       <c r="B16" s="9" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="30" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>9</v>
@@ -1180,13 +1184,13 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>9</v>
@@ -1195,13 +1199,13 @@
     <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>24</v>
@@ -1210,13 +1214,13 @@
     <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>24</v>
@@ -1225,13 +1229,13 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E22" s="3"/>
     </row>
@@ -1244,29 +1248,42 @@
     </row>
     <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="8"/>
-      <c r="B25" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="10" t="s">
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="16"/>
+      <c r="B25" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="28"/>
+      <c r="B26" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="10" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
templates/Surgery/Oppsummering.oet: ny oppsummering Operasjon-forms - behov for logikk.xlsx surgery/Operasjon-forms - behov for logikk.xlsx: oppdatert
</commit_message>
<xml_diff>
--- a/surgery/Operasjon-forms - behov for logikk.xlsx
+++ b/surgery/Operasjon-forms - behov for logikk.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
   <si>
     <t>Arketype</t>
   </si>
@@ -41,15 +41,9 @@
     <t>Dokument/template</t>
   </si>
   <si>
-    <t>Problem/diagnose</t>
-  </si>
-  <si>
     <t>Felt/element</t>
   </si>
   <si>
-    <t>Diagnose</t>
-  </si>
-  <si>
     <t>Estimert knivtid</t>
   </si>
   <si>
@@ -93,9 +87,6 @@
   </si>
   <si>
     <t>Avdekning/incisjon</t>
-  </si>
-  <si>
-    <t>BNAMGR</t>
   </si>
   <si>
     <t>BNA/MGR</t>
@@ -154,15 +145,9 @@
     <t>Re-use. Gjenbruk informasjon fra saken (siste verdi).</t>
   </si>
   <si>
-    <t xml:space="preserve">Re-use. Gjenbruk informasjon fra saken (sdiste verdi). </t>
-  </si>
-  <si>
     <t>Det må vises at informasjonen er innhentet fra en annen plass f.eks. grået ut?</t>
   </si>
   <si>
-    <t>Re-use. Dersom medikament er registrert i operatørvurdering skal det vises som risikofaktor. Er det mulig i fase 1? Hvordan?</t>
-  </si>
-  <si>
     <t>Re-use. Dersom røyking status er satt på røyker skal det vises som risikofaktor? Er det mulig i fase 1? Hvordan?</t>
   </si>
   <si>
@@ -181,12 +166,6 @@
     <t>Beregnet tidsfrist</t>
   </si>
   <si>
-    <t xml:space="preserve">Skal ikke vises i skjema, kun mulighet til å legge til. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">hele Fieldset </t>
-  </si>
-  <si>
     <t>Ønsket helsepsersonell</t>
   </si>
   <si>
@@ -208,21 +187,12 @@
     <t>Kan dette vises slik: syst/diast mmHg?</t>
   </si>
   <si>
-    <t>alt</t>
-  </si>
-  <si>
-    <t>Forcwe min. multiplicity virker ikke. Ønsker at det kun vises som legg til felt.</t>
-  </si>
-  <si>
     <t>Force min multiplicity</t>
   </si>
   <si>
     <t>Får vi dette til å virke også på cluster nivå? Virker ikke nå.</t>
   </si>
   <si>
-    <t>Allergi i versjon 4</t>
-  </si>
-  <si>
     <t>Allergi med betydning i versjon 5</t>
   </si>
   <si>
@@ -233,6 +203,12 @@
   </si>
   <si>
     <t>Reservasjoner med betydning i versjon 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-use. Gjenbruk informasjon fra saken (siste verdi). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-use. Dersom medikament er registrert i operatørvurdering skal det vises som risikofaktor. </t>
   </si>
 </sst>
 </file>
@@ -524,9 +500,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -603,6 +576,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -890,9 +866,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -906,385 +882,340 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="15"/>
+      <c r="B3" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="15"/>
+      <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="C4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="15"/>
+      <c r="B5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="15"/>
+      <c r="B6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="23"/>
+      <c r="B7" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="15"/>
+      <c r="B9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="15"/>
+      <c r="B10" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="15"/>
+      <c r="B11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="15"/>
+      <c r="B12" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="C12" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="24"/>
-      <c r="B9" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="14" t="s">
+      <c r="C16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>67</v>
+      <c r="D16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>9</v>
+        <v>60</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="A21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="15"/>
+      <c r="B22" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="17" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="16"/>
-      <c r="B25" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="28"/>
-      <c r="B26" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>24</v>
+      <c r="A23" s="27"/>
+      <c r="B23" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
surgery/Operasjon-forms - behov for logikk.xlsx: oppdatert templates/Surgery/Beslutningsnotat.v4.oet: startet på nytt for å legge inn lokasjon. Koder ikke ok enda, må rettes før export til opt. anestesi alle: forsøk på problemsløsning. prvisorsikse templates og opts.
</commit_message>
<xml_diff>
--- a/surgery/Operasjon-forms - behov for logikk.xlsx
+++ b/surgery/Operasjon-forms - behov for logikk.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
   <si>
     <t>Arketype</t>
   </si>
@@ -209,6 +209,21 @@
   </si>
   <si>
     <t xml:space="preserve">Re-use. Dersom medikament er registrert i operatørvurdering skal det vises som risikofaktor. </t>
+  </si>
+  <si>
+    <t>Oppsummering</t>
+  </si>
+  <si>
+    <t>Alle arketyper</t>
+  </si>
+  <si>
+    <t>Spørringer må skrives. For alle arketyper gjelder: siste verdi hentes. Unntak: planlagt anestesi. Her må alle verdier hentes. Dvs aestesi 1, 2 og evt. 3. Tooltipp med info om hvem og når dette er skrevet inn. Evt. dokument også?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MGR </t>
+  </si>
+  <si>
+    <t>Anestesi previsitt</t>
   </si>
 </sst>
 </file>
@@ -272,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -485,11 +500,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -579,6 +639,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -868,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1098,7 +1167,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
@@ -1157,7 +1228,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>37</v>
@@ -1170,12 +1241,20 @@
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+    <row r="20" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">

</xml_diff>

<commit_message>
Slettet versjon 2 av operatørvudering for å unngå forvirring. Oppdatert arket med forms logikk
</commit_message>
<xml_diff>
--- a/surgery/Operasjon-forms - behov for logikk.xlsx
+++ b/surgery/Operasjon-forms - behov for logikk.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
   <si>
     <t>Arketype</t>
   </si>
@@ -224,6 +224,18 @@
   </si>
   <si>
     <t>Anestesi previsitt</t>
+  </si>
+  <si>
+    <t>Antibiotikaprofylakse</t>
+  </si>
+  <si>
+    <t>Tromboseprofylakse</t>
+  </si>
+  <si>
+    <t>Medikamenter ved kirurgi</t>
+  </si>
+  <si>
+    <t>Sjekk at lenken virker:)</t>
   </si>
 </sst>
 </file>
@@ -549,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -648,6 +660,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -935,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1136,164 +1151,191 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="23"/>
+      <c r="B13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="23"/>
+      <c r="C14" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C15" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D15" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8" t="s">
+      <c r="E15" s="29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C16" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="E16" s="29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E17" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="31" t="s">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B22" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32" t="s">
+      <c r="C22" s="32"/>
+      <c r="D22" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E22" s="33" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B23" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5" t="s">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E23" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="26" t="s">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="15"/>
+      <c r="B24" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13" t="s">
+      <c r="C24" s="13"/>
+      <c r="D24" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E24" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="27"/>
-      <c r="B23" s="19" t="s">
+    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="27"/>
+      <c r="B25" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28" t="s">
+      <c r="C25" s="28"/>
+      <c r="D25" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E25" s="9" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
openEHR-EHR-EVALUATION.risk.v1.adl: rettet en skrivefeil i norsk oversettelse templates/ Risikovurdering pasient før anestesi.oet: laget section risikovurdering - ikke ferdig enda templates/Sjekkliste anestesi.oet: lagetr section sjekkliste anestesi - ferdig templates/Surgery/Anestesi previsitt v2.oet: laget ny template med sections
</commit_message>
<xml_diff>
--- a/surgery/Operasjon-forms - behov for logikk.xlsx
+++ b/surgery/Operasjon-forms - behov for logikk.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
   <si>
     <t>Arketype</t>
   </si>
@@ -236,6 +236,21 @@
   </si>
   <si>
     <t>Sjekk at lenken virker:)</t>
+  </si>
+  <si>
+    <t>ok:) fikset</t>
+  </si>
+  <si>
+    <t>Lokalisering</t>
+  </si>
+  <si>
+    <t>Omsorgsnivå</t>
+  </si>
+  <si>
+    <t>MGR?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lokalisering av type operasjonssted må hentes her </t>
   </si>
 </sst>
 </file>
@@ -279,7 +294,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,8 +313,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -557,11 +578,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -581,9 +628,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -635,9 +679,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -663,6 +704,27 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -950,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -966,19 +1028,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
     </row>
@@ -995,347 +1057,363 @@
       <c r="D2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
-      <c r="B3" s="20" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="20" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="23"/>
-      <c r="B7" s="24" t="s">
+      <c r="E6" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="37"/>
+      <c r="B8" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C8" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D8" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="E8" s="36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="13" t="s">
+      <c r="E9" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="14"/>
+      <c r="B10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="13" t="s">
+      <c r="E10" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="14"/>
+      <c r="B11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="13" t="s">
+      <c r="E11" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="14"/>
+      <c r="B12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="13" t="s">
+      <c r="E12" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="14"/>
+      <c r="B13" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
-      <c r="B13" s="2" t="s">
+      <c r="E13" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="22"/>
+      <c r="B14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D14" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="C14" s="24" t="s">
+      <c r="E14" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D15" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8" t="s">
+      <c r="E15" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C16" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8" t="s">
+      <c r="E16" s="27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="33"/>
+      <c r="B17" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C17" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="E17" s="27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="E18" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="31" t="s">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B23" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32" t="s">
+      <c r="C23" s="30"/>
+      <c r="D23" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E23" s="31" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B24" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5" t="s">
+      <c r="C24" s="5"/>
+      <c r="D24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
-      <c r="B24" s="26" t="s">
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="14"/>
+      <c r="B25" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13" t="s">
+      <c r="C25" s="12"/>
+      <c r="D25" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E25" s="16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="27"/>
-      <c r="B25" s="19" t="s">
+    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="25"/>
+      <c r="B26" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28" t="s">
+      <c r="C26" s="26"/>
+      <c r="D26" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E26" s="8" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
surgery/Operasjon-forms - behov for logikk.xlsx: oppdatert templates/Surgery/Sjekkliste anestesi.oet: lagt til allergi og omrokkert litt
</commit_message>
<xml_diff>
--- a/surgery/Operasjon-forms - behov for logikk.xlsx
+++ b/surgery/Operasjon-forms - behov for logikk.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
   <si>
     <t>Arketype</t>
   </si>
@@ -127,18 +127,6 @@
     <t>Legg til forklaring i tooltipp som hjelpetekst</t>
   </si>
   <si>
-    <t>Helserisiko annet</t>
-  </si>
-  <si>
-    <t>Risikofaktor</t>
-  </si>
-  <si>
-    <t>Helserisiko medikamenter</t>
-  </si>
-  <si>
-    <t>Medikament</t>
-  </si>
-  <si>
     <t>Evaluering anestesi previsitt</t>
   </si>
   <si>
@@ -148,9 +136,6 @@
     <t>Det må vises at informasjonen er innhentet fra en annen plass f.eks. grået ut?</t>
   </si>
   <si>
-    <t>Re-use. Dersom røyking status er satt på røyker skal det vises som risikofaktor? Er det mulig i fase 1? Hvordan?</t>
-  </si>
-  <si>
     <t>Annet/generelt:</t>
   </si>
   <si>
@@ -208,9 +193,6 @@
     <t xml:space="preserve">Re-use. Gjenbruk informasjon fra saken (siste verdi). </t>
   </si>
   <si>
-    <t xml:space="preserve">Re-use. Dersom medikament er registrert i operatørvurdering skal det vises som risikofaktor. </t>
-  </si>
-  <si>
     <t>Oppsummering</t>
   </si>
   <si>
@@ -251,22 +233,41 @@
   </si>
   <si>
     <t xml:space="preserve">Lokalisering av type operasjonssted må hentes her </t>
+  </si>
+  <si>
+    <t>Tobakksbruk</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Alle</t>
+  </si>
+  <si>
+    <t>Re-use. Gjenburk fra operatørvurdering.</t>
+  </si>
+  <si>
+    <t>Sjekkliste medikasjon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-use. Dersom medikament og kommentar er registrert i operatørvurdering skal det vises som risikofaktor. </t>
+  </si>
+  <si>
+    <t>Helserisiko allergier</t>
+  </si>
+  <si>
+    <t>Stoff og beskrivelse</t>
+  </si>
+  <si>
+    <t>Re-use. Dersom det er fylt ut i operatørvurdering skal det vises her. OBS, jeg ser at jeg har gitt de forskjellige navn, får vi til allikvele. Skal rette dette etter mandag:)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -280,32 +281,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -540,51 +528,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -596,6 +539,41 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -608,123 +586,105 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1012,408 +972,421 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.5546875" style="2"/>
+    <col min="1" max="1" width="23.88671875" style="29" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.5546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.5546875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:5" s="28" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="27" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="18"/>
+      <c r="B8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="19" t="s">
+      <c r="C13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E13" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="21"/>
+      <c r="B17" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="6"/>
+      <c r="B20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
+      <c r="B22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="30"/>
+    </row>
+    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="31"/>
+      <c r="B23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="32"/>
+    </row>
+    <row r="24" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="6"/>
+      <c r="B26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="31"/>
+      <c r="B27" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="12" t="s">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="37"/>
-      <c r="B8" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="36" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
-      <c r="B12" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-      <c r="B14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="33"/>
-      <c r="B17" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="31" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
-      <c r="B25" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="25"/>
-      <c r="B26" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="8" t="s">
+      <c r="E27" s="13" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>